<commit_message>
updates lombok template and validations
</commit_message>
<xml_diff>
--- a/public/Logbook.template.xlsx
+++ b/public/Logbook.template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <workbookProtection workbookPassword="C470" lockStructure="1"/>
   <bookViews>
@@ -2303,7 +2303,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2463,6 +2463,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2819,7 +2831,7 @@
   <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2956,7 +2968,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="L4" s="57"/>
       <c r="M4" s="12"/>
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
@@ -2979,7 +2991,7 @@
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
+      <c r="L5" s="58"/>
       <c r="M5" s="16"/>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
@@ -3002,7 +3014,7 @@
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
+      <c r="L6" s="58"/>
       <c r="M6" s="16"/>
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
@@ -3025,7 +3037,7 @@
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
+      <c r="L7" s="58"/>
       <c r="M7" s="17"/>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
@@ -3049,7 +3061,7 @@
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
+      <c r="L8" s="58"/>
       <c r="M8" s="17"/>
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
@@ -3072,7 +3084,7 @@
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+      <c r="L9" s="58"/>
       <c r="M9" s="17"/>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
@@ -3095,7 +3107,7 @@
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
+      <c r="L10" s="58"/>
       <c r="M10" s="17"/>
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
@@ -3118,7 +3130,7 @@
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
+      <c r="L11" s="58"/>
       <c r="M11" s="17"/>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
@@ -3141,7 +3153,7 @@
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
+      <c r="L12" s="58"/>
       <c r="M12" s="17"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
@@ -3164,7 +3176,7 @@
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
+      <c r="L13" s="58"/>
       <c r="M13" s="17"/>
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
@@ -3187,7 +3199,7 @@
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
+      <c r="L14" s="58"/>
       <c r="M14" s="17"/>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
@@ -3210,7 +3222,7 @@
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
       <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
+      <c r="L15" s="58"/>
       <c r="M15" s="17"/>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
@@ -3233,7 +3245,7 @@
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
+      <c r="L16" s="58"/>
       <c r="M16" s="17"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
@@ -3256,7 +3268,7 @@
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
+      <c r="L17" s="58"/>
       <c r="M17" s="17"/>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
@@ -3279,7 +3291,7 @@
       <c r="I18" s="17"/>
       <c r="J18" s="17"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
+      <c r="L18" s="58"/>
       <c r="M18" s="17"/>
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
@@ -3302,7 +3314,7 @@
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
+      <c r="L19" s="58"/>
       <c r="M19" s="17"/>
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
@@ -3325,7 +3337,7 @@
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
+      <c r="L20" s="58"/>
       <c r="M20" s="17"/>
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
@@ -3348,7 +3360,7 @@
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
       <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
+      <c r="L21" s="58"/>
       <c r="M21" s="17"/>
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
@@ -3371,7 +3383,7 @@
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
+      <c r="L22" s="58"/>
       <c r="M22" s="17"/>
       <c r="N22" s="13"/>
       <c r="O22" s="13"/>
@@ -3394,7 +3406,7 @@
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
+      <c r="L23" s="58"/>
       <c r="M23" s="17"/>
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
@@ -3417,7 +3429,7 @@
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
+      <c r="L24" s="58"/>
       <c r="M24" s="17"/>
       <c r="N24" s="13"/>
       <c r="O24" s="13"/>
@@ -3440,7 +3452,7 @@
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
+      <c r="L25" s="58"/>
       <c r="M25" s="17"/>
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
@@ -3463,7 +3475,7 @@
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
       <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
+      <c r="L26" s="58"/>
       <c r="M26" s="17"/>
       <c r="N26" s="13"/>
       <c r="O26" s="13"/>
@@ -3486,7 +3498,7 @@
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
       <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
+      <c r="L27" s="58"/>
       <c r="M27" s="17"/>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
@@ -3509,7 +3521,7 @@
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
       <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
+      <c r="L28" s="58"/>
       <c r="M28" s="17"/>
       <c r="N28" s="13"/>
       <c r="O28" s="13"/>
@@ -3532,7 +3544,7 @@
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
+      <c r="L29" s="58"/>
       <c r="M29" s="17"/>
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
@@ -3555,7 +3567,7 @@
       <c r="I30" s="17"/>
       <c r="J30" s="17"/>
       <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
+      <c r="L30" s="58"/>
       <c r="M30" s="17"/>
       <c r="N30" s="13"/>
       <c r="O30" s="13"/>
@@ -3578,7 +3590,7 @@
       <c r="I31" s="17"/>
       <c r="J31" s="17"/>
       <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
+      <c r="L31" s="58"/>
       <c r="M31" s="17"/>
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
@@ -3601,7 +3613,7 @@
       <c r="I32" s="17"/>
       <c r="J32" s="17"/>
       <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
+      <c r="L32" s="58"/>
       <c r="M32" s="17"/>
       <c r="N32" s="13"/>
       <c r="O32" s="13"/>
@@ -3624,7 +3636,7 @@
       <c r="I33" s="17"/>
       <c r="J33" s="17"/>
       <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
+      <c r="L33" s="58"/>
       <c r="M33" s="17"/>
       <c r="N33" s="13"/>
       <c r="O33" s="13"/>
@@ -3647,7 +3659,7 @@
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
+      <c r="L34" s="59"/>
       <c r="M34" s="19"/>
       <c r="N34" s="20"/>
       <c r="O34" s="20"/>

</xml_diff>